<commit_message>
- adjustements after first tests, it throws LIN-frames so far
</commit_message>
<xml_diff>
--- a/D5035-51/D5035-51-01/Project Outputs/D5035-51_BOM.xlsx
+++ b/D5035-51/D5035-51-01/Project Outputs/D5035-51_BOM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -97,9 +97,6 @@
     <t xml:space="preserve">SOT23-5</t>
   </si>
   <si>
-    <t xml:space="preserve">do not populate</t>
-  </si>
-  <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
@@ -148,7 +145,7 @@
     <t xml:space="preserve">2k</t>
   </si>
   <si>
-    <t xml:space="preserve">R100, R110, R112, R114, R117, R122, R126</t>
+    <t xml:space="preserve">R100, R110, R112, R114, R122</t>
   </si>
   <si>
     <t xml:space="preserve">C22975</t>
@@ -175,19 +172,16 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
-    <t xml:space="preserve">R111, R113</t>
+    <t xml:space="preserve">R111, R113, R115, R118, R119, R124, R127, R128</t>
   </si>
   <si>
     <t xml:space="preserve">C21190</t>
   </si>
   <si>
-    <t xml:space="preserve">4k7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R115, R118, R119, R124, R127, R128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23162</t>
+    <t xml:space="preserve">680R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R117, R126</t>
   </si>
   <si>
     <t xml:space="preserve">1k/500mW</t>
@@ -299,11 +293,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -319,12 +314,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -409,7 +398,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,11 +411,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,11 +423,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,14 +511,15 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,404 +529,370 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="6" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="6" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="D29" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>